<commit_message>
changes in docs, planning ( user stories, system stories )
</commit_message>
<xml_diff>
--- a/docs/Planning.xlsx
+++ b/docs/Planning.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17571"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17726"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>User Stories</t>
   </si>
@@ -37,12 +37,75 @@
       <t>njmo</t>
     </r>
   </si>
+  <si>
+    <t>as a user I want to:</t>
+  </si>
+  <si>
+    <t>get information about specific resource</t>
+  </si>
+  <si>
+    <t>register myself to get scheduled data about resource</t>
+  </si>
+  <si>
+    <t>get information when resource state changed</t>
+  </si>
+  <si>
+    <t>set specific action on resource state change</t>
+  </si>
+  <si>
+    <t>specify list of chained actions on reactions</t>
+  </si>
+  <si>
+    <t>System stories</t>
+  </si>
+  <si>
+    <t>as a system component:</t>
+  </si>
+  <si>
+    <t>I want to queue myself as a waiter and be notified by event</t>
+  </si>
+  <si>
+    <t>I want to send response to multiple waiters</t>
+  </si>
+  <si>
+    <t>Component Name</t>
+  </si>
+  <si>
+    <t>Nanny</t>
+  </si>
+  <si>
+    <t>EventQueue,Handler</t>
+  </si>
+  <si>
+    <t>I want to schedule event when specific amount of time elapsed</t>
+  </si>
+  <si>
+    <t>Nanny,Timeout</t>
+  </si>
+  <si>
+    <t>I want to return response to waiter</t>
+  </si>
+  <si>
+    <t>get information about changing state of event</t>
+  </si>
+  <si>
+    <t>be able to receive and handle connection request</t>
+  </si>
+  <si>
+    <t>be able to handle more than one connection in time</t>
+  </si>
+  <si>
+    <t>be able to send message to specific user</t>
+  </si>
+  <si>
+    <t>be able to wait for response of pushed event</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -69,8 +132,41 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -89,8 +185,23 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -113,17 +224,47 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -132,9 +273,28 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="4" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="3" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Calculation" xfId="2" builtinId="22"/>
+    <cellStyle name="Explanatory Text" xfId="4" builtinId="53"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note" xfId="3" builtinId="10"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -415,321 +575,678 @@
   <dimension ref="E2:U35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="M17" sqref="M17:R17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="9" max="9" width="35.5703125" customWidth="1"/>
+    <col min="18" max="18" width="13.140625" customWidth="1"/>
+    <col min="19" max="19" width="19.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="2" spans="5:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I2" s="4" t="s">
+    <row r="2" spans="5:21" ht="15" customHeight="1">
+      <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-    </row>
-    <row r="3" spans="5:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
-      <c r="U3" s="5"/>
-    </row>
-    <row r="4" spans="5:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I4" s="5"/>
-      <c r="J4" s="5"/>
-      <c r="K4" s="5"/>
-      <c r="L4" s="5"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="5"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
-      <c r="U4" s="5"/>
-    </row>
-    <row r="7" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E7" s="3" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+    </row>
+    <row r="3" spans="5:21" ht="15" customHeight="1">
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="U3" s="3"/>
+    </row>
+    <row r="4" spans="5:21" ht="15" customHeight="1">
+      <c r="I4" s="3"/>
+      <c r="J4" s="3"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+      <c r="M4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="R4" s="3"/>
+      <c r="S4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="U4" s="3"/>
+    </row>
+    <row r="6" spans="5:21">
+      <c r="E6" t="s">
+        <v>2</v>
+      </c>
+      <c r="L6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="5:21">
+      <c r="E7" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-    </row>
-    <row r="8" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E8" s="2">
+      <c r="F7" s="4"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="L7" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="6"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="7" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="5:21">
+      <c r="E8" s="9">
         <v>1</v>
       </c>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
-      <c r="H8" s="1"/>
-      <c r="I8" s="1"/>
-    </row>
-    <row r="9" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E9" s="2">
+      <c r="F8" s="10" t="s">
+        <v>3</v>
+      </c>
+      <c r="G8" s="10"/>
+      <c r="H8" s="10"/>
+      <c r="I8" s="10"/>
+      <c r="L8" s="8">
+        <v>1</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="N8" s="10"/>
+      <c r="O8" s="10"/>
+      <c r="P8" s="10"/>
+      <c r="Q8" s="10"/>
+      <c r="R8" s="10"/>
+      <c r="S8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="5:21">
+      <c r="E9" s="9">
         <v>2</v>
       </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-    </row>
-    <row r="10" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E10" s="2">
+      <c r="F9" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="10"/>
+      <c r="H9" s="10"/>
+      <c r="I9" s="10"/>
+      <c r="L9" s="8">
+        <v>2</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="N9" s="10"/>
+      <c r="O9" s="10"/>
+      <c r="P9" s="10"/>
+      <c r="Q9" s="10"/>
+      <c r="R9" s="10"/>
+      <c r="S9" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="5:21">
+      <c r="E10" s="9">
         <v>3</v>
       </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
-      <c r="H10" s="1"/>
-      <c r="I10" s="1"/>
-    </row>
-    <row r="11" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E11" s="2">
+      <c r="F10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="10"/>
+      <c r="H10" s="10"/>
+      <c r="I10" s="10"/>
+      <c r="L10" s="8">
+        <v>3</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="N10" s="10"/>
+      <c r="O10" s="10"/>
+      <c r="P10" s="10"/>
+      <c r="Q10" s="10"/>
+      <c r="R10" s="10"/>
+      <c r="S10" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="11" spans="5:21">
+      <c r="E11" s="9">
         <v>4</v>
       </c>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
-      <c r="H11" s="1"/>
-      <c r="I11" s="1"/>
-    </row>
-    <row r="12" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E12" s="2">
+      <c r="F11" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="10"/>
+      <c r="H11" s="10"/>
+      <c r="I11" s="10"/>
+      <c r="L11" s="8">
+        <v>4</v>
+      </c>
+      <c r="M11" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="N11" s="10"/>
+      <c r="O11" s="10"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="10"/>
+      <c r="R11" s="10"/>
+    </row>
+    <row r="12" spans="5:21">
+      <c r="E12" s="9">
         <v>5</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-    </row>
-    <row r="13" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E13" s="2">
+      <c r="F12" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="10"/>
+      <c r="L12" s="8">
+        <v>5</v>
+      </c>
+      <c r="M12" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="N12" s="10"/>
+      <c r="O12" s="10"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="10"/>
+      <c r="R12" s="10"/>
+    </row>
+    <row r="13" spans="5:21">
+      <c r="E13" s="9">
         <v>6</v>
       </c>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
-    </row>
-    <row r="14" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E14" s="2">
+      <c r="L13" s="8">
+        <v>6</v>
+      </c>
+      <c r="M13" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="N13" s="10"/>
+      <c r="O13" s="10"/>
+      <c r="P13" s="10"/>
+      <c r="Q13" s="10"/>
+      <c r="R13" s="10"/>
+    </row>
+    <row r="14" spans="5:21">
+      <c r="E14" s="9">
         <v>7</v>
       </c>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
-    </row>
-    <row r="15" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E15" s="2">
+      <c r="L14" s="8">
+        <v>7</v>
+      </c>
+      <c r="M14" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="N14" s="10"/>
+      <c r="O14" s="10"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="10"/>
+      <c r="R14" s="10"/>
+    </row>
+    <row r="15" spans="5:21">
+      <c r="E15" s="9">
         <v>8</v>
       </c>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
       <c r="I15" s="1"/>
-    </row>
-    <row r="16" spans="5:21" x14ac:dyDescent="0.25">
-      <c r="E16" s="2">
+      <c r="L15" s="8">
+        <v>8</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="N15" s="10"/>
+      <c r="O15" s="10"/>
+      <c r="P15" s="10"/>
+      <c r="Q15" s="10"/>
+      <c r="R15" s="10"/>
+    </row>
+    <row r="16" spans="5:21">
+      <c r="E16" s="9">
         <v>9</v>
       </c>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
       <c r="I16" s="1"/>
-    </row>
-    <row r="17" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E17" s="2">
+      <c r="L16" s="8">
+        <v>9</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="10"/>
+      <c r="O16" s="10"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="10"/>
+      <c r="R16" s="10"/>
+    </row>
+    <row r="17" spans="5:18">
+      <c r="E17" s="9">
         <v>10</v>
       </c>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
       <c r="I17" s="1"/>
-    </row>
-    <row r="18" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E18" s="2">
+      <c r="L17" s="8">
+        <v>10</v>
+      </c>
+      <c r="M17" s="5"/>
+      <c r="N17" s="5"/>
+      <c r="O17" s="5"/>
+      <c r="P17" s="5"/>
+      <c r="Q17" s="5"/>
+      <c r="R17" s="5"/>
+    </row>
+    <row r="18" spans="5:18">
+      <c r="E18" s="9">
         <v>11</v>
       </c>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
-    </row>
-    <row r="19" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E19" s="2">
+      <c r="L18" s="8">
+        <v>11</v>
+      </c>
+      <c r="M18" s="5"/>
+      <c r="N18" s="5"/>
+      <c r="O18" s="5"/>
+      <c r="P18" s="5"/>
+      <c r="Q18" s="5"/>
+      <c r="R18" s="5"/>
+    </row>
+    <row r="19" spans="5:18">
+      <c r="E19" s="9">
         <v>12</v>
       </c>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
       <c r="I19" s="1"/>
-    </row>
-    <row r="20" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E20" s="2">
+      <c r="L19" s="8">
+        <v>12</v>
+      </c>
+      <c r="M19" s="5"/>
+      <c r="N19" s="5"/>
+      <c r="O19" s="5"/>
+      <c r="P19" s="5"/>
+      <c r="Q19" s="5"/>
+      <c r="R19" s="5"/>
+    </row>
+    <row r="20" spans="5:18">
+      <c r="E20" s="9">
         <v>13</v>
       </c>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
       <c r="I20" s="1"/>
-    </row>
-    <row r="21" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E21" s="2">
+      <c r="L20" s="8">
+        <v>13</v>
+      </c>
+      <c r="M20" s="5"/>
+      <c r="N20" s="5"/>
+      <c r="O20" s="5"/>
+      <c r="P20" s="5"/>
+      <c r="Q20" s="5"/>
+      <c r="R20" s="5"/>
+    </row>
+    <row r="21" spans="5:18">
+      <c r="E21" s="9">
         <v>14</v>
       </c>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
       <c r="I21" s="1"/>
-    </row>
-    <row r="22" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E22" s="2">
+      <c r="L21" s="8">
+        <v>14</v>
+      </c>
+      <c r="M21" s="5"/>
+      <c r="N21" s="5"/>
+      <c r="O21" s="5"/>
+      <c r="P21" s="5"/>
+      <c r="Q21" s="5"/>
+      <c r="R21" s="5"/>
+    </row>
+    <row r="22" spans="5:18">
+      <c r="E22" s="9">
         <v>15</v>
       </c>
       <c r="F22" s="1"/>
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
       <c r="I22" s="1"/>
-    </row>
-    <row r="23" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E23" s="2">
+      <c r="L22" s="8">
+        <v>15</v>
+      </c>
+      <c r="M22" s="5"/>
+      <c r="N22" s="5"/>
+      <c r="O22" s="5"/>
+      <c r="P22" s="5"/>
+      <c r="Q22" s="5"/>
+      <c r="R22" s="5"/>
+    </row>
+    <row r="23" spans="5:18">
+      <c r="E23" s="9">
         <v>16</v>
       </c>
       <c r="F23" s="1"/>
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
       <c r="I23" s="1"/>
-    </row>
-    <row r="24" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E24" s="2">
+      <c r="L23" s="8">
+        <v>16</v>
+      </c>
+      <c r="M23" s="5"/>
+      <c r="N23" s="5"/>
+      <c r="O23" s="5"/>
+      <c r="P23" s="5"/>
+      <c r="Q23" s="5"/>
+      <c r="R23" s="5"/>
+    </row>
+    <row r="24" spans="5:18">
+      <c r="E24" s="9">
         <v>17</v>
       </c>
       <c r="F24" s="1"/>
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
       <c r="I24" s="1"/>
-    </row>
-    <row r="25" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E25" s="2">
+      <c r="L24" s="8">
+        <v>17</v>
+      </c>
+      <c r="M24" s="5"/>
+      <c r="N24" s="5"/>
+      <c r="O24" s="5"/>
+      <c r="P24" s="5"/>
+      <c r="Q24" s="5"/>
+      <c r="R24" s="5"/>
+    </row>
+    <row r="25" spans="5:18">
+      <c r="E25" s="9">
         <v>18</v>
       </c>
       <c r="F25" s="1"/>
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
       <c r="I25" s="1"/>
-    </row>
-    <row r="26" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E26" s="2">
+      <c r="L25" s="8">
+        <v>18</v>
+      </c>
+      <c r="M25" s="5"/>
+      <c r="N25" s="5"/>
+      <c r="O25" s="5"/>
+      <c r="P25" s="5"/>
+      <c r="Q25" s="5"/>
+      <c r="R25" s="5"/>
+    </row>
+    <row r="26" spans="5:18">
+      <c r="E26" s="9">
         <v>19</v>
       </c>
       <c r="F26" s="1"/>
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
       <c r="I26" s="1"/>
-    </row>
-    <row r="27" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E27" s="2">
+      <c r="L26" s="8">
+        <v>19</v>
+      </c>
+      <c r="M26" s="5"/>
+      <c r="N26" s="5"/>
+      <c r="O26" s="5"/>
+      <c r="P26" s="5"/>
+      <c r="Q26" s="5"/>
+      <c r="R26" s="5"/>
+    </row>
+    <row r="27" spans="5:18">
+      <c r="E27" s="9">
         <v>20</v>
       </c>
       <c r="F27" s="1"/>
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
       <c r="I27" s="1"/>
-    </row>
-    <row r="28" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E28" s="2">
+      <c r="L27" s="8">
+        <v>20</v>
+      </c>
+      <c r="M27" s="5"/>
+      <c r="N27" s="5"/>
+      <c r="O27" s="5"/>
+      <c r="P27" s="5"/>
+      <c r="Q27" s="5"/>
+      <c r="R27" s="5"/>
+    </row>
+    <row r="28" spans="5:18">
+      <c r="E28" s="9">
         <v>21</v>
       </c>
       <c r="F28" s="1"/>
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
       <c r="I28" s="1"/>
-    </row>
-    <row r="29" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E29" s="2">
+      <c r="L28" s="8">
+        <v>21</v>
+      </c>
+      <c r="M28" s="5"/>
+      <c r="N28" s="5"/>
+      <c r="O28" s="5"/>
+      <c r="P28" s="5"/>
+      <c r="Q28" s="5"/>
+      <c r="R28" s="5"/>
+    </row>
+    <row r="29" spans="5:18">
+      <c r="E29" s="9">
         <v>22</v>
       </c>
       <c r="F29" s="1"/>
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
       <c r="I29" s="1"/>
-    </row>
-    <row r="30" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E30" s="2">
+      <c r="L29" s="8">
+        <v>22</v>
+      </c>
+      <c r="M29" s="5"/>
+      <c r="N29" s="5"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+    </row>
+    <row r="30" spans="5:18">
+      <c r="E30" s="9">
         <v>23</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
       <c r="I30" s="1"/>
-    </row>
-    <row r="31" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E31" s="2">
+      <c r="L30" s="8">
+        <v>23</v>
+      </c>
+      <c r="M30" s="5"/>
+      <c r="N30" s="5"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+    </row>
+    <row r="31" spans="5:18">
+      <c r="E31" s="9">
         <v>24</v>
       </c>
       <c r="F31" s="1"/>
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
       <c r="I31" s="1"/>
-    </row>
-    <row r="32" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E32" s="2">
+      <c r="L31" s="8">
+        <v>24</v>
+      </c>
+      <c r="M31" s="5"/>
+      <c r="N31" s="5"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+    </row>
+    <row r="32" spans="5:18">
+      <c r="E32" s="9">
         <v>25</v>
       </c>
       <c r="F32" s="1"/>
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
       <c r="I32" s="1"/>
-    </row>
-    <row r="33" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E33" s="2">
+      <c r="L32" s="8">
+        <v>25</v>
+      </c>
+      <c r="M32" s="5"/>
+      <c r="N32" s="5"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+    </row>
+    <row r="33" spans="5:18">
+      <c r="E33" s="9">
         <v>26</v>
       </c>
       <c r="F33" s="1"/>
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
       <c r="I33" s="1"/>
-    </row>
-    <row r="34" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E34" s="2">
+      <c r="L33" s="8">
+        <v>26</v>
+      </c>
+      <c r="M33" s="5"/>
+      <c r="N33" s="5"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+    </row>
+    <row r="34" spans="5:18">
+      <c r="E34" s="9">
         <v>27</v>
       </c>
       <c r="F34" s="1"/>
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
       <c r="I34" s="1"/>
-    </row>
-    <row r="35" spans="5:9" x14ac:dyDescent="0.25">
-      <c r="E35" s="2">
+      <c r="L34" s="8">
+        <v>27</v>
+      </c>
+      <c r="M34" s="5"/>
+      <c r="N34" s="5"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+    </row>
+    <row r="35" spans="5:18">
+      <c r="E35" s="9">
         <v>28</v>
       </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
+      <c r="L35" s="8">
+        <v>28</v>
+      </c>
+      <c r="M35" s="5"/>
+      <c r="N35" s="5"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="30">
+  <mergeCells count="59">
+    <mergeCell ref="M34:R34"/>
+    <mergeCell ref="M35:R35"/>
+    <mergeCell ref="M29:R29"/>
+    <mergeCell ref="M30:R30"/>
+    <mergeCell ref="M31:R31"/>
+    <mergeCell ref="M32:R32"/>
+    <mergeCell ref="M33:R33"/>
+    <mergeCell ref="M24:R24"/>
+    <mergeCell ref="M25:R25"/>
+    <mergeCell ref="M26:R26"/>
+    <mergeCell ref="M27:R27"/>
+    <mergeCell ref="M28:R28"/>
+    <mergeCell ref="M19:R19"/>
+    <mergeCell ref="M20:R20"/>
+    <mergeCell ref="M21:R21"/>
+    <mergeCell ref="M22:R22"/>
+    <mergeCell ref="M23:R23"/>
+    <mergeCell ref="F12:I12"/>
+    <mergeCell ref="F11:I11"/>
+    <mergeCell ref="F10:I10"/>
+    <mergeCell ref="L7:R7"/>
+    <mergeCell ref="M8:R8"/>
+    <mergeCell ref="M9:R9"/>
+    <mergeCell ref="M10:R10"/>
+    <mergeCell ref="M11:R11"/>
+    <mergeCell ref="M12:R12"/>
+    <mergeCell ref="M13:R13"/>
+    <mergeCell ref="M14:R14"/>
+    <mergeCell ref="M15:R15"/>
+    <mergeCell ref="M16:R16"/>
+    <mergeCell ref="M17:R17"/>
+    <mergeCell ref="M18:R18"/>
+    <mergeCell ref="F23:I23"/>
+    <mergeCell ref="F24:I24"/>
+    <mergeCell ref="F25:I25"/>
+    <mergeCell ref="F26:I26"/>
+    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="F14:I14"/>
+    <mergeCell ref="F15:I15"/>
+    <mergeCell ref="F16:I16"/>
+    <mergeCell ref="E7:I7"/>
+    <mergeCell ref="F8:I8"/>
+    <mergeCell ref="F9:I9"/>
     <mergeCell ref="F33:I33"/>
     <mergeCell ref="F34:I34"/>
     <mergeCell ref="F35:I35"/>
@@ -746,20 +1263,6 @@
     <mergeCell ref="F20:I20"/>
     <mergeCell ref="F21:I21"/>
     <mergeCell ref="F22:I22"/>
-    <mergeCell ref="E7:I7"/>
-    <mergeCell ref="F8:I8"/>
-    <mergeCell ref="F9:I9"/>
-    <mergeCell ref="F10:I10"/>
-    <mergeCell ref="F11:I11"/>
-    <mergeCell ref="F23:I23"/>
-    <mergeCell ref="F24:I24"/>
-    <mergeCell ref="F25:I25"/>
-    <mergeCell ref="F26:I26"/>
-    <mergeCell ref="F13:I13"/>
-    <mergeCell ref="F14:I14"/>
-    <mergeCell ref="F15:I15"/>
-    <mergeCell ref="F16:I16"/>
-    <mergeCell ref="F12:I12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>